<commit_message>
amend table pm11, add column6
</commit_message>
<xml_diff>
--- a/predict_dat1.xlsx
+++ b/predict_dat1.xlsx
@@ -3275,16 +3275,16 @@
         <v>62</v>
       </c>
       <c r="E112" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F112" t="n">
-        <v>29.03</v>
+        <v>30.65</v>
       </c>
       <c r="G112" t="n">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H112" t="n">
-        <v>1480</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="113">
@@ -3301,16 +3301,16 @@
         <v>62</v>
       </c>
       <c r="E113" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F113" t="n">
-        <v>35.48</v>
+        <v>37.1</v>
       </c>
       <c r="G113" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H113" t="n">
-        <v>1519</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="114">
@@ -3327,16 +3327,16 @@
         <v>62</v>
       </c>
       <c r="E114" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F114" t="n">
-        <v>32.26</v>
+        <v>33.87</v>
       </c>
       <c r="G114" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H114" t="n">
-        <v>1557</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="115">
@@ -3353,16 +3353,16 @@
         <v>62</v>
       </c>
       <c r="E115" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F115" t="n">
-        <v>30.65</v>
+        <v>32.26</v>
       </c>
       <c r="G115" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H115" t="n">
-        <v>1597</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="116">
@@ -3379,16 +3379,16 @@
         <v>62</v>
       </c>
       <c r="E116" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F116" t="n">
-        <v>19.35</v>
+        <v>20.97</v>
       </c>
       <c r="G116" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H116" t="n">
-        <v>1625</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="117">
@@ -3414,7 +3414,7 @@
         <v>7</v>
       </c>
       <c r="H117" t="n">
-        <v>1632</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="118">
@@ -3440,7 +3440,7 @@
         <v>1</v>
       </c>
       <c r="H118" t="n">
-        <v>1633</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="119">
@@ -3457,16 +3457,16 @@
         <v>64</v>
       </c>
       <c r="E119" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F119" t="n">
-        <v>35.94</v>
+        <v>39.06</v>
       </c>
       <c r="G119" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H119" t="n">
-        <v>1693</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="120">
@@ -3492,7 +3492,7 @@
         <v>28</v>
       </c>
       <c r="H120" t="n">
-        <v>1721</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="121">
@@ -3509,16 +3509,16 @@
         <v>68</v>
       </c>
       <c r="E121" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F121" t="n">
-        <v>30.88</v>
+        <v>33.82</v>
       </c>
       <c r="G121" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H121" t="n">
-        <v>1758</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="122">
@@ -3535,16 +3535,16 @@
         <v>68</v>
       </c>
       <c r="E122" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F122" t="n">
-        <v>22.06</v>
+        <v>23.53</v>
       </c>
       <c r="G122" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H122" t="n">
-        <v>1790</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="123">
@@ -3561,16 +3561,16 @@
         <v>68</v>
       </c>
       <c r="E123" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F123" t="n">
-        <v>11.76</v>
+        <v>14.71</v>
       </c>
       <c r="G123" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H123" t="n">
-        <v>1803</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="124">
@@ -3587,16 +3587,16 @@
         <v>68</v>
       </c>
       <c r="E124" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F124" t="n">
-        <v>10.29</v>
+        <v>11.76</v>
       </c>
       <c r="G124" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H124" t="n">
-        <v>1810</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="125">
@@ -3622,7 +3622,7 @@
         <v>4</v>
       </c>
       <c r="H125" t="n">
-        <v>1814</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="126">
@@ -3639,16 +3639,16 @@
         <v>69</v>
       </c>
       <c r="E126" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F126" t="n">
-        <v>15.94</v>
+        <v>18.84</v>
       </c>
       <c r="G126" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H126" t="n">
-        <v>1836</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="127">
@@ -3665,16 +3665,16 @@
         <v>70</v>
       </c>
       <c r="E127" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F127" t="n">
-        <v>20</v>
+        <v>24.29</v>
       </c>
       <c r="G127" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H127" t="n">
-        <v>1856</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="128">
@@ -3691,16 +3691,68 @@
         <v>70</v>
       </c>
       <c r="E128" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F128" t="n">
-        <v>1.43</v>
+        <v>14.29</v>
       </c>
       <c r="G128" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="H128" t="n">
-        <v>1857</v>
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>45071</v>
+      </c>
+      <c r="B129" t="n">
+        <v>21</v>
+      </c>
+      <c r="C129" t="n">
+        <v>2</v>
+      </c>
+      <c r="D129" t="n">
+        <v>72</v>
+      </c>
+      <c r="E129" t="n">
+        <v>18</v>
+      </c>
+      <c r="F129" t="n">
+        <v>25</v>
+      </c>
+      <c r="G129" t="n">
+        <v>32</v>
+      </c>
+      <c r="H129" t="n">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>45072</v>
+      </c>
+      <c r="B130" t="n">
+        <v>21</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" t="n">
+        <v>72</v>
+      </c>
+      <c r="E130" t="n">
+        <v>4</v>
+      </c>
+      <c r="F130" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="G130" t="n">
+        <v>6</v>
+      </c>
+      <c r="H130" t="n">
+        <v>1957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>